<commit_message>
[JH] 25. Sound, BuildTest
</commit_message>
<xml_diff>
--- a/Chain.of.Heroes/Tools/data/BossMonster_Dragon.xlsx
+++ b/Chain.of.Heroes/Tools/data/BossMonster_Dragon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junha\OneDrive\문서\GitHub\Chain_Of_Heroes\Chain.of.Heroes\Tools\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOJIN\Desktop\졸작\데이터테이블\몬스터\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336A6E44-5879-4644-97E4-A45DC063BB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D18891-B4BE-40E2-81C4-A719D4C24A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dragon" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="77">
   <si>
     <t>Int</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -124,6 +124,14 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>몬스터 등급</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster_Rank</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>몬스터 레벨</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -160,6 +168,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>MonsterRank</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>사룡</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -168,32 +180,129 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t># 사룡 레벨 40</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>마법</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t># 사룡 레벨 2</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 3</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 4</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 5</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 6</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 7</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 8</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 9</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 10</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 11</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 12</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 13</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 14</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 15</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 16</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 17</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 18</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 19</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 20</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 21</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 22</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 23</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 24</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 25</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 26</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 27</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 28</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 29</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 30</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 31</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 32</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 33</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 34</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 35</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 36</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 37</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 38</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 39</t>
+  </si>
+  <si>
+    <t># 사룡 레벨 40</t>
+  </si>
+  <si>
     <t>UnitProperty</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MonsterRank</t>
-  </si>
-  <si>
-    <t>몬스터 등급</t>
-  </si>
-  <si>
-    <t>Monster_Rank</t>
-  </si>
-  <si>
-    <t>보스 몬스터</t>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -778,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -841,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>2</v>
@@ -862,10 +971,10 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -879,7 +988,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>9</v>
@@ -891,10 +1000,10 @@
         <v>13</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>14</v>
@@ -909,10 +1018,10 @@
         <v>20</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -923,10 +1032,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>7</v>
@@ -938,10 +1047,10 @@
         <v>12</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>15</v>
@@ -956,10 +1065,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -967,22 +1076,22 @@
         <v>20150001</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D5" s="17">
         <v>1</v>
       </c>
       <c r="E5" s="17">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F5" s="17">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G5" s="17">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="H5" s="17">
         <v>15</v>
@@ -1002,11 +1111,11 @@
       <c r="M5" s="17">
         <v>1</v>
       </c>
-      <c r="N5" s="17" t="s">
-        <v>39</v>
+      <c r="N5" s="17">
+        <v>2</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1014,46 +1123,1949 @@
         <v>20150002</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="17">
+        <v>2</v>
+      </c>
+      <c r="E6" s="17">
+        <f>ROUNDDOWN(E5*1.1,0)</f>
+        <v>93</v>
+      </c>
+      <c r="F6" s="17">
+        <f>ROUNDDOWN(F5*1.1,0)</f>
+        <v>44</v>
+      </c>
+      <c r="G6" s="17">
+        <f>ROUNDDOWN(G5*1.05,0)</f>
+        <v>1575</v>
+      </c>
+      <c r="H6" s="17">
+        <v>15</v>
+      </c>
+      <c r="I6" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J6" s="17">
+        <v>2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>5</v>
+      </c>
+      <c r="L6" s="17">
+        <v>3</v>
+      </c>
+      <c r="M6" s="17">
+        <v>1</v>
+      </c>
+      <c r="N6" s="17">
+        <v>2</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>20150003</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="17">
+        <v>3</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" ref="E7:E44" si="0">ROUNDDOWN(E6*1.1,0)</f>
+        <v>102</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" ref="F7:F44" si="1">ROUNDDOWN(F6*1.1,0)</f>
+        <v>48</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" ref="G7:G44" si="2">ROUNDDOWN(G6*1.05,0)</f>
+        <v>1653</v>
+      </c>
+      <c r="H7" s="17">
+        <v>15</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J7" s="17">
+        <v>2</v>
+      </c>
+      <c r="K7" s="17">
+        <v>5</v>
+      </c>
+      <c r="L7" s="17">
+        <v>3</v>
+      </c>
+      <c r="M7" s="17">
+        <v>1</v>
+      </c>
+      <c r="N7" s="17">
+        <v>2</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <v>20150004</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="17">
+        <v>4</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="2"/>
+        <v>1735</v>
+      </c>
+      <c r="H8" s="17">
+        <v>15</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J8" s="17">
+        <v>2</v>
+      </c>
+      <c r="K8" s="17">
+        <v>5</v>
+      </c>
+      <c r="L8" s="17">
+        <v>3</v>
+      </c>
+      <c r="M8" s="17">
+        <v>1</v>
+      </c>
+      <c r="N8" s="17">
+        <v>2</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <v>20150005</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="17">
+        <v>5</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="F9" s="17">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="2"/>
+        <v>1821</v>
+      </c>
+      <c r="H9" s="17">
+        <v>15</v>
+      </c>
+      <c r="I9" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J9" s="17">
+        <v>2</v>
+      </c>
+      <c r="K9" s="17">
+        <v>5</v>
+      </c>
+      <c r="L9" s="17">
+        <v>3</v>
+      </c>
+      <c r="M9" s="17">
+        <v>1</v>
+      </c>
+      <c r="N9" s="17">
+        <v>2</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
+        <v>20150006</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="17">
+        <v>6</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="F10" s="17">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="2"/>
+        <v>1912</v>
+      </c>
+      <c r="H10" s="17">
+        <v>15</v>
+      </c>
+      <c r="I10" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J10" s="17">
+        <v>2</v>
+      </c>
+      <c r="K10" s="17">
+        <v>5</v>
+      </c>
+      <c r="L10" s="17">
+        <v>3</v>
+      </c>
+      <c r="M10" s="17">
+        <v>1</v>
+      </c>
+      <c r="N10" s="17">
+        <v>2</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
+        <v>20150007</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="17">
+        <v>7</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="2"/>
+        <v>2007</v>
+      </c>
+      <c r="H11" s="17">
+        <v>15</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J11" s="17">
+        <v>2</v>
+      </c>
+      <c r="K11" s="17">
+        <v>5</v>
+      </c>
+      <c r="L11" s="17">
+        <v>3</v>
+      </c>
+      <c r="M11" s="17">
+        <v>1</v>
+      </c>
+      <c r="N11" s="17">
+        <v>2</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <v>20150008</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="17">
+        <v>8</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="2"/>
+        <v>2107</v>
+      </c>
+      <c r="H12" s="17">
+        <v>15</v>
+      </c>
+      <c r="I12" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J12" s="17">
+        <v>2</v>
+      </c>
+      <c r="K12" s="17">
+        <v>5</v>
+      </c>
+      <c r="L12" s="17">
+        <v>3</v>
+      </c>
+      <c r="M12" s="17">
+        <v>1</v>
+      </c>
+      <c r="N12" s="17">
+        <v>2</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <v>20150009</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="17">
+        <v>9</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="2"/>
+        <v>2212</v>
+      </c>
+      <c r="H13" s="17">
+        <v>15</v>
+      </c>
+      <c r="I13" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J13" s="17">
+        <v>2</v>
+      </c>
+      <c r="K13" s="17">
+        <v>5</v>
+      </c>
+      <c r="L13" s="17">
+        <v>3</v>
+      </c>
+      <c r="M13" s="17">
+        <v>1</v>
+      </c>
+      <c r="N13" s="17">
+        <v>2</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="17">
+        <v>20150010</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="17">
+        <v>10</v>
+      </c>
+      <c r="E14" s="17">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="2"/>
+        <v>2322</v>
+      </c>
+      <c r="H14" s="17">
+        <v>15</v>
+      </c>
+      <c r="I14" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J14" s="17">
+        <v>2</v>
+      </c>
+      <c r="K14" s="17">
+        <v>5</v>
+      </c>
+      <c r="L14" s="17">
+        <v>3</v>
+      </c>
+      <c r="M14" s="17">
+        <v>1</v>
+      </c>
+      <c r="N14" s="17">
+        <v>2</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="17">
+        <v>20150011</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="17">
+        <v>11</v>
+      </c>
+      <c r="E15" s="17">
+        <f t="shared" si="0"/>
+        <v>214</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="2"/>
+        <v>2438</v>
+      </c>
+      <c r="H15" s="17">
+        <v>15</v>
+      </c>
+      <c r="I15" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J15" s="17">
+        <v>2</v>
+      </c>
+      <c r="K15" s="17">
+        <v>5</v>
+      </c>
+      <c r="L15" s="17">
+        <v>3</v>
+      </c>
+      <c r="M15" s="17">
+        <v>1</v>
+      </c>
+      <c r="N15" s="17">
+        <v>2</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
+        <v>20150012</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="17">
+        <v>12</v>
+      </c>
+      <c r="E16" s="17">
+        <f t="shared" si="0"/>
+        <v>235</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="2"/>
+        <v>2559</v>
+      </c>
+      <c r="H16" s="17">
+        <v>15</v>
+      </c>
+      <c r="I16" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J16" s="17">
+        <v>2</v>
+      </c>
+      <c r="K16" s="17">
+        <v>5</v>
+      </c>
+      <c r="L16" s="17">
+        <v>3</v>
+      </c>
+      <c r="M16" s="17">
+        <v>1</v>
+      </c>
+      <c r="N16" s="17">
+        <v>2</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="17">
+        <v>20150013</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="17">
+        <v>13</v>
+      </c>
+      <c r="E17" s="17">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="F17" s="17">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="2"/>
+        <v>2686</v>
+      </c>
+      <c r="H17" s="17">
+        <v>15</v>
+      </c>
+      <c r="I17" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J17" s="17">
+        <v>2</v>
+      </c>
+      <c r="K17" s="17">
+        <v>5</v>
+      </c>
+      <c r="L17" s="17">
+        <v>3</v>
+      </c>
+      <c r="M17" s="17">
+        <v>1</v>
+      </c>
+      <c r="N17" s="17">
+        <v>2</v>
+      </c>
+      <c r="O17" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>20150014</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="17">
+        <v>14</v>
+      </c>
+      <c r="E18" s="17">
+        <f t="shared" si="0"/>
+        <v>283</v>
+      </c>
+      <c r="F18" s="17">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="2"/>
+        <v>2820</v>
+      </c>
+      <c r="H18" s="17">
+        <v>15</v>
+      </c>
+      <c r="I18" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J18" s="17">
+        <v>2</v>
+      </c>
+      <c r="K18" s="17">
+        <v>5</v>
+      </c>
+      <c r="L18" s="17">
+        <v>3</v>
+      </c>
+      <c r="M18" s="17">
+        <v>1</v>
+      </c>
+      <c r="N18" s="17">
+        <v>2</v>
+      </c>
+      <c r="O18" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="17">
+        <v>20150015</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="17">
+        <v>15</v>
+      </c>
+      <c r="E19" s="17">
+        <f t="shared" si="0"/>
+        <v>311</v>
+      </c>
+      <c r="F19" s="17">
+        <f t="shared" si="1"/>
+        <v>139</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="2"/>
+        <v>2961</v>
+      </c>
+      <c r="H19" s="17">
+        <v>15</v>
+      </c>
+      <c r="I19" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J19" s="17">
+        <v>2</v>
+      </c>
+      <c r="K19" s="17">
+        <v>5</v>
+      </c>
+      <c r="L19" s="17">
+        <v>3</v>
+      </c>
+      <c r="M19" s="17">
+        <v>1</v>
+      </c>
+      <c r="N19" s="17">
+        <v>2</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="17">
+        <v>20150016</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="17">
+        <v>16</v>
+      </c>
+      <c r="E20" s="17">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" si="1"/>
+        <v>152</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="2"/>
+        <v>3109</v>
+      </c>
+      <c r="H20" s="17">
+        <v>15</v>
+      </c>
+      <c r="I20" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J20" s="17">
+        <v>2</v>
+      </c>
+      <c r="K20" s="17">
+        <v>5</v>
+      </c>
+      <c r="L20" s="17">
+        <v>3</v>
+      </c>
+      <c r="M20" s="17">
+        <v>1</v>
+      </c>
+      <c r="N20" s="17">
+        <v>2</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="17">
+        <v>20150017</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="17">
+        <v>17</v>
+      </c>
+      <c r="E21" s="17">
+        <f t="shared" si="0"/>
+        <v>376</v>
+      </c>
+      <c r="F21" s="17">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="2"/>
+        <v>3264</v>
+      </c>
+      <c r="H21" s="17">
+        <v>15</v>
+      </c>
+      <c r="I21" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J21" s="17">
+        <v>2</v>
+      </c>
+      <c r="K21" s="17">
+        <v>5</v>
+      </c>
+      <c r="L21" s="17">
+        <v>3</v>
+      </c>
+      <c r="M21" s="17">
+        <v>1</v>
+      </c>
+      <c r="N21" s="17">
+        <v>2</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="17">
+        <v>20150018</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="17">
+        <v>18</v>
+      </c>
+      <c r="E22" s="17">
+        <f t="shared" si="0"/>
+        <v>413</v>
+      </c>
+      <c r="F22" s="17">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="G22" s="17">
+        <f t="shared" si="2"/>
+        <v>3427</v>
+      </c>
+      <c r="H22" s="17">
+        <v>15</v>
+      </c>
+      <c r="I22" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J22" s="17">
+        <v>2</v>
+      </c>
+      <c r="K22" s="17">
+        <v>5</v>
+      </c>
+      <c r="L22" s="17">
+        <v>3</v>
+      </c>
+      <c r="M22" s="17">
+        <v>1</v>
+      </c>
+      <c r="N22" s="17">
+        <v>2</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="17">
+        <v>20150019</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="17">
+        <v>19</v>
+      </c>
+      <c r="E23" s="17">
+        <f t="shared" si="0"/>
+        <v>454</v>
+      </c>
+      <c r="F23" s="17">
+        <f t="shared" si="1"/>
+        <v>201</v>
+      </c>
+      <c r="G23" s="17">
+        <f t="shared" si="2"/>
+        <v>3598</v>
+      </c>
+      <c r="H23" s="17">
+        <v>15</v>
+      </c>
+      <c r="I23" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J23" s="17">
+        <v>2</v>
+      </c>
+      <c r="K23" s="17">
+        <v>5</v>
+      </c>
+      <c r="L23" s="17">
+        <v>3</v>
+      </c>
+      <c r="M23" s="17">
+        <v>1</v>
+      </c>
+      <c r="N23" s="17">
+        <v>2</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="17">
+        <v>20150020</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="17">
+        <v>20</v>
+      </c>
+      <c r="E24" s="17">
+        <f t="shared" si="0"/>
+        <v>499</v>
+      </c>
+      <c r="F24" s="17">
+        <f t="shared" si="1"/>
+        <v>221</v>
+      </c>
+      <c r="G24" s="17">
+        <f t="shared" si="2"/>
+        <v>3777</v>
+      </c>
+      <c r="H24" s="17">
+        <v>15</v>
+      </c>
+      <c r="I24" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J24" s="17">
+        <v>2</v>
+      </c>
+      <c r="K24" s="17">
+        <v>5</v>
+      </c>
+      <c r="L24" s="17">
+        <v>3</v>
+      </c>
+      <c r="M24" s="17">
+        <v>1</v>
+      </c>
+      <c r="N24" s="17">
+        <v>2</v>
+      </c>
+      <c r="O24" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="17">
+        <v>20150021</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="17">
+        <v>21</v>
+      </c>
+      <c r="E25" s="17">
+        <f t="shared" si="0"/>
+        <v>548</v>
+      </c>
+      <c r="F25" s="17">
+        <f t="shared" si="1"/>
+        <v>243</v>
+      </c>
+      <c r="G25" s="17">
+        <f t="shared" si="2"/>
+        <v>3965</v>
+      </c>
+      <c r="H25" s="17">
+        <v>15</v>
+      </c>
+      <c r="I25" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J25" s="17">
+        <v>2</v>
+      </c>
+      <c r="K25" s="17">
+        <v>5</v>
+      </c>
+      <c r="L25" s="17">
+        <v>3</v>
+      </c>
+      <c r="M25" s="17">
+        <v>1</v>
+      </c>
+      <c r="N25" s="17">
+        <v>2</v>
+      </c>
+      <c r="O25" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="17">
+        <v>20150022</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="17">
+        <v>22</v>
+      </c>
+      <c r="E26" s="17">
+        <f t="shared" si="0"/>
+        <v>602</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="1"/>
+        <v>267</v>
+      </c>
+      <c r="G26" s="17">
+        <f t="shared" si="2"/>
+        <v>4163</v>
+      </c>
+      <c r="H26" s="17">
+        <v>15</v>
+      </c>
+      <c r="I26" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J26" s="17">
+        <v>2</v>
+      </c>
+      <c r="K26" s="17">
+        <v>5</v>
+      </c>
+      <c r="L26" s="17">
+        <v>3</v>
+      </c>
+      <c r="M26" s="17">
+        <v>1</v>
+      </c>
+      <c r="N26" s="17">
+        <v>2</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="17">
+        <v>20150023</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="17">
+        <v>23</v>
+      </c>
+      <c r="E27" s="17">
+        <f t="shared" si="0"/>
+        <v>662</v>
+      </c>
+      <c r="F27" s="17">
+        <f t="shared" si="1"/>
+        <v>293</v>
+      </c>
+      <c r="G27" s="17">
+        <f t="shared" si="2"/>
+        <v>4371</v>
+      </c>
+      <c r="H27" s="17">
+        <v>15</v>
+      </c>
+      <c r="I27" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J27" s="17">
+        <v>2</v>
+      </c>
+      <c r="K27" s="17">
+        <v>5</v>
+      </c>
+      <c r="L27" s="17">
+        <v>3</v>
+      </c>
+      <c r="M27" s="17">
+        <v>1</v>
+      </c>
+      <c r="N27" s="17">
+        <v>2</v>
+      </c>
+      <c r="O27" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="17">
+        <v>20150024</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="17">
+        <v>24</v>
+      </c>
+      <c r="E28" s="17">
+        <f t="shared" si="0"/>
+        <v>728</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" si="1"/>
+        <v>322</v>
+      </c>
+      <c r="G28" s="17">
+        <f t="shared" si="2"/>
+        <v>4589</v>
+      </c>
+      <c r="H28" s="17">
+        <v>15</v>
+      </c>
+      <c r="I28" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J28" s="17">
+        <v>2</v>
+      </c>
+      <c r="K28" s="17">
+        <v>5</v>
+      </c>
+      <c r="L28" s="17">
+        <v>3</v>
+      </c>
+      <c r="M28" s="17">
+        <v>1</v>
+      </c>
+      <c r="N28" s="17">
+        <v>2</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="17">
+        <v>20150025</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="17">
+        <v>25</v>
+      </c>
+      <c r="E29" s="17">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="1"/>
+        <v>354</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" si="2"/>
+        <v>4818</v>
+      </c>
+      <c r="H29" s="17">
+        <v>15</v>
+      </c>
+      <c r="I29" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J29" s="17">
+        <v>2</v>
+      </c>
+      <c r="K29" s="17">
+        <v>5</v>
+      </c>
+      <c r="L29" s="17">
+        <v>3</v>
+      </c>
+      <c r="M29" s="17">
+        <v>1</v>
+      </c>
+      <c r="N29" s="17">
+        <v>2</v>
+      </c>
+      <c r="O29" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="17">
+        <v>20150026</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="17">
+        <v>26</v>
+      </c>
+      <c r="E30" s="17">
+        <f t="shared" si="0"/>
+        <v>880</v>
+      </c>
+      <c r="F30" s="17">
+        <f t="shared" si="1"/>
+        <v>389</v>
+      </c>
+      <c r="G30" s="17">
+        <f t="shared" si="2"/>
+        <v>5058</v>
+      </c>
+      <c r="H30" s="17">
+        <v>15</v>
+      </c>
+      <c r="I30" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J30" s="17">
+        <v>2</v>
+      </c>
+      <c r="K30" s="17">
+        <v>5</v>
+      </c>
+      <c r="L30" s="17">
+        <v>3</v>
+      </c>
+      <c r="M30" s="17">
+        <v>1</v>
+      </c>
+      <c r="N30" s="17">
+        <v>2</v>
+      </c>
+      <c r="O30" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="17">
+        <v>20150027</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="17">
+        <v>27</v>
+      </c>
+      <c r="E31" s="17">
+        <f t="shared" si="0"/>
+        <v>968</v>
+      </c>
+      <c r="F31" s="17">
+        <f t="shared" si="1"/>
+        <v>427</v>
+      </c>
+      <c r="G31" s="17">
+        <f t="shared" si="2"/>
+        <v>5310</v>
+      </c>
+      <c r="H31" s="17">
+        <v>15</v>
+      </c>
+      <c r="I31" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J31" s="17">
+        <v>2</v>
+      </c>
+      <c r="K31" s="17">
+        <v>5</v>
+      </c>
+      <c r="L31" s="17">
+        <v>3</v>
+      </c>
+      <c r="M31" s="17">
+        <v>1</v>
+      </c>
+      <c r="N31" s="17">
+        <v>2</v>
+      </c>
+      <c r="O31" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="17">
+        <v>20150028</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="17">
+        <v>28</v>
+      </c>
+      <c r="E32" s="17">
+        <f t="shared" si="0"/>
+        <v>1064</v>
+      </c>
+      <c r="F32" s="17">
+        <f t="shared" si="1"/>
+        <v>469</v>
+      </c>
+      <c r="G32" s="17">
+        <f t="shared" si="2"/>
+        <v>5575</v>
+      </c>
+      <c r="H32" s="17">
+        <v>15</v>
+      </c>
+      <c r="I32" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J32" s="17">
+        <v>2</v>
+      </c>
+      <c r="K32" s="17">
+        <v>5</v>
+      </c>
+      <c r="L32" s="17">
+        <v>3</v>
+      </c>
+      <c r="M32" s="17">
+        <v>1</v>
+      </c>
+      <c r="N32" s="17">
+        <v>2</v>
+      </c>
+      <c r="O32" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="17">
+        <v>20150029</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="17">
+        <v>29</v>
+      </c>
+      <c r="E33" s="17">
+        <f t="shared" si="0"/>
+        <v>1170</v>
+      </c>
+      <c r="F33" s="17">
+        <f t="shared" si="1"/>
+        <v>515</v>
+      </c>
+      <c r="G33" s="17">
+        <f t="shared" si="2"/>
+        <v>5853</v>
+      </c>
+      <c r="H33" s="17">
+        <v>15</v>
+      </c>
+      <c r="I33" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J33" s="17">
+        <v>2</v>
+      </c>
+      <c r="K33" s="17">
+        <v>5</v>
+      </c>
+      <c r="L33" s="17">
+        <v>3</v>
+      </c>
+      <c r="M33" s="17">
+        <v>1</v>
+      </c>
+      <c r="N33" s="17">
+        <v>2</v>
+      </c>
+      <c r="O33" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="17">
+        <v>20150030</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="17">
+        <v>30</v>
+      </c>
+      <c r="E34" s="17">
+        <f t="shared" si="0"/>
+        <v>1287</v>
+      </c>
+      <c r="F34" s="17">
+        <f t="shared" si="1"/>
+        <v>566</v>
+      </c>
+      <c r="G34" s="17">
+        <f t="shared" si="2"/>
+        <v>6145</v>
+      </c>
+      <c r="H34" s="17">
+        <v>15</v>
+      </c>
+      <c r="I34" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J34" s="17">
+        <v>2</v>
+      </c>
+      <c r="K34" s="17">
+        <v>5</v>
+      </c>
+      <c r="L34" s="17">
+        <v>3</v>
+      </c>
+      <c r="M34" s="17">
+        <v>1</v>
+      </c>
+      <c r="N34" s="17">
+        <v>2</v>
+      </c>
+      <c r="O34" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="17">
+        <v>20150031</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="17">
+        <v>31</v>
+      </c>
+      <c r="E35" s="17">
+        <f t="shared" si="0"/>
+        <v>1415</v>
+      </c>
+      <c r="F35" s="17">
+        <f t="shared" si="1"/>
+        <v>622</v>
+      </c>
+      <c r="G35" s="17">
+        <f t="shared" si="2"/>
+        <v>6452</v>
+      </c>
+      <c r="H35" s="17">
+        <v>15</v>
+      </c>
+      <c r="I35" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J35" s="17">
+        <v>2</v>
+      </c>
+      <c r="K35" s="17">
+        <v>5</v>
+      </c>
+      <c r="L35" s="17">
+        <v>3</v>
+      </c>
+      <c r="M35" s="17">
+        <v>1</v>
+      </c>
+      <c r="N35" s="17">
+        <v>2</v>
+      </c>
+      <c r="O35" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="17">
+        <v>20150032</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="17">
+        <v>32</v>
+      </c>
+      <c r="E36" s="17">
+        <f t="shared" si="0"/>
+        <v>1556</v>
+      </c>
+      <c r="F36" s="17">
+        <f t="shared" si="1"/>
+        <v>684</v>
+      </c>
+      <c r="G36" s="17">
+        <f t="shared" si="2"/>
+        <v>6774</v>
+      </c>
+      <c r="H36" s="17">
+        <v>15</v>
+      </c>
+      <c r="I36" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J36" s="17">
+        <v>2</v>
+      </c>
+      <c r="K36" s="17">
+        <v>5</v>
+      </c>
+      <c r="L36" s="17">
+        <v>3</v>
+      </c>
+      <c r="M36" s="17">
+        <v>1</v>
+      </c>
+      <c r="N36" s="17">
+        <v>2</v>
+      </c>
+      <c r="O36" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="17">
+        <v>20150033</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="17">
         <v>33</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="17">
+      <c r="E37" s="17">
+        <f t="shared" si="0"/>
+        <v>1711</v>
+      </c>
+      <c r="F37" s="17">
+        <f t="shared" si="1"/>
+        <v>752</v>
+      </c>
+      <c r="G37" s="17">
+        <f t="shared" si="2"/>
+        <v>7112</v>
+      </c>
+      <c r="H37" s="17">
+        <v>15</v>
+      </c>
+      <c r="I37" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J37" s="17">
+        <v>2</v>
+      </c>
+      <c r="K37" s="17">
+        <v>5</v>
+      </c>
+      <c r="L37" s="17">
+        <v>3</v>
+      </c>
+      <c r="M37" s="17">
+        <v>1</v>
+      </c>
+      <c r="N37" s="17">
+        <v>2</v>
+      </c>
+      <c r="O37" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="17">
+        <v>20150034</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="17">
+        <v>34</v>
+      </c>
+      <c r="E38" s="17">
+        <f t="shared" si="0"/>
+        <v>1882</v>
+      </c>
+      <c r="F38" s="17">
+        <f t="shared" si="1"/>
+        <v>827</v>
+      </c>
+      <c r="G38" s="17">
+        <f t="shared" si="2"/>
+        <v>7467</v>
+      </c>
+      <c r="H38" s="17">
+        <v>15</v>
+      </c>
+      <c r="I38" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J38" s="17">
+        <v>2</v>
+      </c>
+      <c r="K38" s="17">
+        <v>5</v>
+      </c>
+      <c r="L38" s="17">
+        <v>3</v>
+      </c>
+      <c r="M38" s="17">
+        <v>1</v>
+      </c>
+      <c r="N38" s="17">
+        <v>2</v>
+      </c>
+      <c r="O38" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="17">
+        <v>20150035</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="17">
+        <v>35</v>
+      </c>
+      <c r="E39" s="17">
+        <f t="shared" si="0"/>
+        <v>2070</v>
+      </c>
+      <c r="F39" s="17">
+        <f t="shared" si="1"/>
+        <v>909</v>
+      </c>
+      <c r="G39" s="17">
+        <f t="shared" si="2"/>
+        <v>7840</v>
+      </c>
+      <c r="H39" s="17">
+        <v>15</v>
+      </c>
+      <c r="I39" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J39" s="17">
+        <v>2</v>
+      </c>
+      <c r="K39" s="17">
+        <v>5</v>
+      </c>
+      <c r="L39" s="17">
+        <v>3</v>
+      </c>
+      <c r="M39" s="17">
+        <v>1</v>
+      </c>
+      <c r="N39" s="17">
+        <v>2</v>
+      </c>
+      <c r="O39" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="17">
+        <v>20150036</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="17">
+        <v>36</v>
+      </c>
+      <c r="E40" s="17">
+        <f t="shared" si="0"/>
+        <v>2277</v>
+      </c>
+      <c r="F40" s="17">
+        <f t="shared" si="1"/>
+        <v>999</v>
+      </c>
+      <c r="G40" s="17">
+        <f t="shared" si="2"/>
+        <v>8232</v>
+      </c>
+      <c r="H40" s="17">
+        <v>15</v>
+      </c>
+      <c r="I40" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J40" s="17">
+        <v>2</v>
+      </c>
+      <c r="K40" s="17">
+        <v>5</v>
+      </c>
+      <c r="L40" s="17">
+        <v>3</v>
+      </c>
+      <c r="M40" s="17">
+        <v>1</v>
+      </c>
+      <c r="N40" s="17">
+        <v>2</v>
+      </c>
+      <c r="O40" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="17">
+        <v>20150037</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="17">
+        <v>37</v>
+      </c>
+      <c r="E41" s="17">
+        <f t="shared" si="0"/>
+        <v>2504</v>
+      </c>
+      <c r="F41" s="17">
+        <f t="shared" si="1"/>
+        <v>1098</v>
+      </c>
+      <c r="G41" s="17">
+        <f t="shared" si="2"/>
+        <v>8643</v>
+      </c>
+      <c r="H41" s="17">
+        <v>15</v>
+      </c>
+      <c r="I41" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J41" s="17">
+        <v>2</v>
+      </c>
+      <c r="K41" s="17">
+        <v>5</v>
+      </c>
+      <c r="L41" s="17">
+        <v>3</v>
+      </c>
+      <c r="M41" s="17">
+        <v>1</v>
+      </c>
+      <c r="N41" s="17">
+        <v>2</v>
+      </c>
+      <c r="O41" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="17">
+        <v>20150038</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="17">
+        <v>38</v>
+      </c>
+      <c r="E42" s="17">
+        <f t="shared" si="0"/>
+        <v>2754</v>
+      </c>
+      <c r="F42" s="17">
+        <f t="shared" si="1"/>
+        <v>1207</v>
+      </c>
+      <c r="G42" s="17">
+        <f t="shared" si="2"/>
+        <v>9075</v>
+      </c>
+      <c r="H42" s="17">
+        <v>15</v>
+      </c>
+      <c r="I42" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J42" s="17">
+        <v>2</v>
+      </c>
+      <c r="K42" s="17">
+        <v>5</v>
+      </c>
+      <c r="L42" s="17">
+        <v>3</v>
+      </c>
+      <c r="M42" s="17">
+        <v>1</v>
+      </c>
+      <c r="N42" s="17">
+        <v>2</v>
+      </c>
+      <c r="O42" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="17">
+        <v>20150039</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="17">
+        <v>39</v>
+      </c>
+      <c r="E43" s="17">
+        <f t="shared" si="0"/>
+        <v>3029</v>
+      </c>
+      <c r="F43" s="17">
+        <f t="shared" si="1"/>
+        <v>1327</v>
+      </c>
+      <c r="G43" s="17">
+        <f t="shared" si="2"/>
+        <v>9528</v>
+      </c>
+      <c r="H43" s="17">
+        <v>15</v>
+      </c>
+      <c r="I43" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J43" s="17">
+        <v>2</v>
+      </c>
+      <c r="K43" s="17">
+        <v>5</v>
+      </c>
+      <c r="L43" s="17">
+        <v>3</v>
+      </c>
+      <c r="M43" s="17">
+        <v>1</v>
+      </c>
+      <c r="N43" s="17">
+        <v>2</v>
+      </c>
+      <c r="O43" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="17">
+        <v>20150040</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="17">
         <v>40</v>
       </c>
-      <c r="E6" s="17">
-        <v>2000</v>
-      </c>
-      <c r="F6" s="17">
-        <v>1000</v>
-      </c>
-      <c r="G6" s="17">
-        <v>7500</v>
-      </c>
-      <c r="H6" s="17">
-        <v>15</v>
-      </c>
-      <c r="I6" s="17">
-        <v>1.3</v>
-      </c>
-      <c r="J6" s="17">
-        <v>2</v>
-      </c>
-      <c r="K6" s="17">
-        <v>5</v>
-      </c>
-      <c r="L6" s="17">
-        <v>3</v>
-      </c>
-      <c r="M6" s="17">
-        <v>1</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>34</v>
+      <c r="E44" s="17">
+        <f t="shared" si="0"/>
+        <v>3331</v>
+      </c>
+      <c r="F44" s="17">
+        <f t="shared" si="1"/>
+        <v>1459</v>
+      </c>
+      <c r="G44" s="17">
+        <f t="shared" si="2"/>
+        <v>10004</v>
+      </c>
+      <c r="H44" s="17">
+        <v>15</v>
+      </c>
+      <c r="I44" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J44" s="17">
+        <v>2</v>
+      </c>
+      <c r="K44" s="17">
+        <v>5</v>
+      </c>
+      <c r="L44" s="17">
+        <v>3</v>
+      </c>
+      <c r="M44" s="17">
+        <v>1</v>
+      </c>
+      <c r="N44" s="17">
+        <v>2</v>
+      </c>
+      <c r="O44" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>